<commit_message>
pre proc updated : no accents and spaces
</commit_message>
<xml_diff>
--- a/MP2/results.xlsx
+++ b/MP2/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1630,6 +1630,574 @@
         <v>2000</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ComplementNB</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.7397804972804973</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.8303198887343533</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>L - TF - NLe - 2G - F2000</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1761283874511719</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>ComplementNB()</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>(1, 2)</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>TF</t>
+        </is>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>F_CL</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ComplementNB</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.7934702797202797</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.8831710709318498</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>L - C - NLe - 2G - F2000 - No Acc</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>0.2726867198944092</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>ComplementNB()</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>(1, 2)</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>F_CL</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ComplementNB</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.7932915695415695</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.8831710709318498</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L - C - NLe - 2G - F2000 - Punc w space</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>0.1486952304840088</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>ComplementNB()</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>(1, 2)</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>F_CL</t>
+        </is>
+      </c>
+      <c r="P22" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ComplementNB</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.6340540015540015</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>NL - B - NLe - 2G</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>0.4496505260467529</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>ComplementNB()</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>(1, 2)</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Bin</t>
+        </is>
+      </c>
+      <c r="K23" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23" t="b">
+        <v>0</v>
+      </c>
+      <c r="M23" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23" t="b">
+        <v>0</v>
+      </c>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ComplementNB</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.6576991064491065</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>NL - C - NLe - 2G</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>0.4078330993652344</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>ComplementNB()</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>(1, 2)</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" t="b">
+        <v>0</v>
+      </c>
+      <c r="M24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ComplementNB</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0.8034741647241648</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.885952712100139</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Big test</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>0.1550121307373047</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>ComplementNB()</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>(1, 2)</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="K25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25" t="b">
+        <v>1</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>F_CL</t>
+        </is>
+      </c>
+      <c r="P25" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ComplementNB</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.8061120823620824</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.8929068150208623</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Big test- BIN</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>0.1614856719970703</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>ComplementNB()</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>(1, 2)</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Bin</t>
+        </is>
+      </c>
+      <c r="K26" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26" t="b">
+        <v>1</v>
+      </c>
+      <c r="M26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>F_CL</t>
+        </is>
+      </c>
+      <c r="P26" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ComplementNB</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.8079254079254079</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.8984700973574409</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Big test- BIN - NL</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>0.1612675189971924</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>ComplementNB()</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>(1, 2)</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Bin</t>
+        </is>
+      </c>
+      <c r="K27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>F_CL</t>
+        </is>
+      </c>
+      <c r="P27" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ComplementNB</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.8063908313908315</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.8901251738525731</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Big test- Count - NL</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>0.1819298267364502</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>ComplementNB()</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>(1, 2)</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="K28" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>F_CL</t>
+        </is>
+      </c>
+      <c r="P28" t="n">
+        <v>2000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>